<commit_message>
Add times Round 3
</commit_message>
<xml_diff>
--- a/11/USQ-Cup/ROCHESTER_TEXAS.xlsx
+++ b/11/USQ-Cup/ROCHESTER_TEXAS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raghu\quidditch\live-stats\11\USQ-Cup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{118475D8-8653-43E6-8589-B4E889998AC4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{620E3D4F-D971-4091-9CB6-34C8C5DEAE92}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="9800" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1200" windowWidth="7120" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="85">
   <si>
     <t>A</t>
   </si>
@@ -59,9 +61,6 @@
   </si>
   <si>
     <t>TL</t>
-  </si>
-  <si>
-    <t>?</t>
   </si>
   <si>
     <t>TC</t>
@@ -172,13 +171,121 @@
     <t>S</t>
   </si>
   <si>
-    <t>G</t>
-  </si>
-  <si>
     <t>MADDISON JORDAN</t>
   </si>
   <si>
     <t>JUSTIN KING</t>
+  </si>
+  <si>
+    <t>0044</t>
+  </si>
+  <si>
+    <t>0145</t>
+  </si>
+  <si>
+    <t>0211</t>
+  </si>
+  <si>
+    <t>0238</t>
+  </si>
+  <si>
+    <t>0255</t>
+  </si>
+  <si>
+    <t>0418</t>
+  </si>
+  <si>
+    <t>0440</t>
+  </si>
+  <si>
+    <t>0511</t>
+  </si>
+  <si>
+    <t>0537</t>
+  </si>
+  <si>
+    <t>0638</t>
+  </si>
+  <si>
+    <t>0705</t>
+  </si>
+  <si>
+    <t>0732</t>
+  </si>
+  <si>
+    <t>0741</t>
+  </si>
+  <si>
+    <t>0826</t>
+  </si>
+  <si>
+    <t>0900</t>
+  </si>
+  <si>
+    <t>0910</t>
+  </si>
+  <si>
+    <t>0944</t>
+  </si>
+  <si>
+    <t>1024</t>
+  </si>
+  <si>
+    <t>1030</t>
+  </si>
+  <si>
+    <t>1101</t>
+  </si>
+  <si>
+    <t>1138</t>
+  </si>
+  <si>
+    <t>1233</t>
+  </si>
+  <si>
+    <t>1326</t>
+  </si>
+  <si>
+    <t>1417</t>
+  </si>
+  <si>
+    <t>1451</t>
+  </si>
+  <si>
+    <t>1500</t>
+  </si>
+  <si>
+    <t>1535</t>
+  </si>
+  <si>
+    <t>1543</t>
+  </si>
+  <si>
+    <t>1614</t>
+  </si>
+  <si>
+    <t>1648</t>
+  </si>
+  <si>
+    <t>1715</t>
+  </si>
+  <si>
+    <t>1816</t>
+  </si>
+  <si>
+    <t>1908</t>
+  </si>
+  <si>
+    <t>1935</t>
+  </si>
+  <si>
+    <t>2008</t>
+  </si>
+  <si>
+    <t>2025</t>
+  </si>
+  <si>
+    <t>2026</t>
   </si>
 </sst>
 </file>
@@ -460,7 +567,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -468,20 +583,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -703,8 +810,8 @@
   </sheetPr>
   <dimension ref="A1:Z994"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="77" workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+    <sheetView tabSelected="1" topLeftCell="H8" zoomScale="77" workbookViewId="0">
+      <selection activeCell="Q19" sqref="Q19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -733,21 +840,21 @@
     <row r="1" spans="1:26" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="26"/>
-      <c r="N1" s="26"/>
-      <c r="O1" s="25"/>
-      <c r="P1" s="26"/>
-      <c r="Q1" s="26"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
       <c r="R1" s="2"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
@@ -760,140 +867,140 @@
     </row>
     <row r="2" spans="1:26" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="J2" s="16"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="23">
+      <c r="J2" s="20"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="19">
         <f>COUNTIFS(A:A,"G*") + COUNTIFS(G:G,"G*")+COUNTIFS(M:M,"G*")+COUNTIFS(S:S,"G*")</f>
         <v>7</v>
       </c>
-      <c r="M2" s="16"/>
-      <c r="N2" s="17"/>
-      <c r="O2" s="24" t="str">
+      <c r="M2" s="20"/>
+      <c r="N2" s="21"/>
+      <c r="O2" s="25" t="str">
         <f>IF(COUNTIF($A$7:$X$59,"RCA"),"*","")&amp;IF(COUNTIF($A$7:$X$59,"OCA"),"^","")&amp;IF(COUNTIF($R$7:$X$59,"2CA"),"!","")</f>
         <v>*</v>
       </c>
-      <c r="P2" s="16"/>
-      <c r="Q2" s="17"/>
-      <c r="R2" s="15" t="str">
+      <c r="P2" s="20"/>
+      <c r="Q2" s="21"/>
+      <c r="R2" s="26" t="str">
         <f>CONCATENATE(LEN(O2)*30+L2*10,O2)</f>
         <v>100*</v>
       </c>
-      <c r="S2" s="16"/>
-      <c r="T2" s="16"/>
-      <c r="U2" s="16"/>
-      <c r="V2" s="16"/>
-      <c r="W2" s="17"/>
+      <c r="S2" s="20"/>
+      <c r="T2" s="20"/>
+      <c r="U2" s="20"/>
+      <c r="V2" s="20"/>
+      <c r="W2" s="21"/>
       <c r="X2" s="1"/>
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
     </row>
     <row r="3" spans="1:26" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="B3" s="22"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="19"/>
-      <c r="K3" s="20"/>
-      <c r="L3" s="18"/>
-      <c r="M3" s="19"/>
-      <c r="N3" s="20"/>
-      <c r="O3" s="18"/>
-      <c r="P3" s="19"/>
-      <c r="Q3" s="20"/>
-      <c r="R3" s="18"/>
-      <c r="S3" s="19"/>
-      <c r="T3" s="19"/>
-      <c r="U3" s="19"/>
-      <c r="V3" s="19"/>
-      <c r="W3" s="20"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="22"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="24"/>
+      <c r="L3" s="22"/>
+      <c r="M3" s="23"/>
+      <c r="N3" s="24"/>
+      <c r="O3" s="22"/>
+      <c r="P3" s="23"/>
+      <c r="Q3" s="24"/>
+      <c r="R3" s="22"/>
+      <c r="S3" s="23"/>
+      <c r="T3" s="23"/>
+      <c r="U3" s="23"/>
+      <c r="V3" s="23"/>
+      <c r="W3" s="24"/>
       <c r="X3" s="1"/>
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
     </row>
     <row r="4" spans="1:26" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="23"/>
-      <c r="J4" s="16"/>
-      <c r="K4" s="17"/>
-      <c r="L4" s="23">
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="19">
         <f>COUNTIFS(D:D,"G*")+COUNTIFS(J:J,"G*")+COUNTIFS(P:P,"G*")+COUNTIFS(V:V,"G*")</f>
         <v>9</v>
       </c>
-      <c r="M4" s="16"/>
-      <c r="N4" s="17"/>
-      <c r="O4" s="24" t="str">
+      <c r="M4" s="20"/>
+      <c r="N4" s="21"/>
+      <c r="O4" s="25" t="str">
         <f>IF(COUNTIF($A$7:$R$59,"RCB"),"*","")&amp;IF(COUNTIF($A$7:$R$59,"OCB"),"^","")&amp;IF(COUNTIF($A$7:$R$59,"2CB"),"!","")</f>
         <v/>
       </c>
-      <c r="P4" s="16"/>
-      <c r="Q4" s="17"/>
-      <c r="R4" s="15" t="str">
+      <c r="P4" s="20"/>
+      <c r="Q4" s="21"/>
+      <c r="R4" s="26" t="str">
         <f>CONCATENATE(LEN(O4)*30+L4*10,O4)</f>
         <v>90</v>
       </c>
-      <c r="S4" s="16"/>
-      <c r="T4" s="16"/>
-      <c r="U4" s="16"/>
-      <c r="V4" s="16"/>
-      <c r="W4" s="17"/>
+      <c r="S4" s="20"/>
+      <c r="T4" s="20"/>
+      <c r="U4" s="20"/>
+      <c r="V4" s="20"/>
+      <c r="W4" s="21"/>
       <c r="X4" s="1"/>
       <c r="Y4" s="1"/>
       <c r="Z4" s="1"/>
     </row>
     <row r="5" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="B5" s="22"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="19"/>
-      <c r="K5" s="20"/>
-      <c r="L5" s="18"/>
-      <c r="M5" s="19"/>
-      <c r="N5" s="20"/>
-      <c r="O5" s="18"/>
-      <c r="P5" s="19"/>
-      <c r="Q5" s="20"/>
-      <c r="R5" s="18"/>
-      <c r="S5" s="19"/>
-      <c r="T5" s="19"/>
-      <c r="U5" s="19"/>
-      <c r="V5" s="19"/>
-      <c r="W5" s="20"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="24"/>
+      <c r="L5" s="22"/>
+      <c r="M5" s="23"/>
+      <c r="N5" s="24"/>
+      <c r="O5" s="22"/>
+      <c r="P5" s="23"/>
+      <c r="Q5" s="24"/>
+      <c r="R5" s="22"/>
+      <c r="S5" s="23"/>
+      <c r="T5" s="23"/>
+      <c r="U5" s="23"/>
+      <c r="V5" s="23"/>
+      <c r="W5" s="24"/>
       <c r="X5" s="1"/>
       <c r="Y5" s="1"/>
       <c r="Z5" s="1"/>
@@ -931,44 +1038,60 @@
       <c r="B7" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="5"/>
+      <c r="C7" s="5" t="s">
+        <v>48</v>
+      </c>
       <c r="D7" s="6"/>
       <c r="E7" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="8"/>
+      <c r="F7" s="8" t="s">
+        <v>49</v>
+      </c>
       <c r="G7" s="3"/>
       <c r="H7" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="I7" s="5"/>
+      <c r="I7" s="5" t="s">
+        <v>50</v>
+      </c>
       <c r="J7" s="6"/>
       <c r="K7" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="L7" s="8"/>
+      <c r="L7" s="8" t="s">
+        <v>51</v>
+      </c>
       <c r="M7" s="3"/>
       <c r="N7" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="O7" s="5"/>
+      <c r="O7" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="P7" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q7" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="R7" s="8"/>
+      <c r="R7" s="8" t="s">
+        <v>53</v>
+      </c>
       <c r="S7" s="3"/>
       <c r="T7" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="U7" s="5"/>
+      <c r="U7" s="5" t="s">
+        <v>54</v>
+      </c>
       <c r="V7" s="6"/>
       <c r="W7" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="X7" s="8"/>
+      <c r="X7" s="8" t="s">
+        <v>55</v>
+      </c>
       <c r="Y7" s="1"/>
       <c r="Z7" s="1"/>
     </row>
@@ -989,7 +1112,7 @@
         <v>95</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G8" s="9" t="s">
         <v>6</v>
@@ -1069,44 +1192,60 @@
       <c r="B10" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="5"/>
+      <c r="C10" s="5" t="s">
+        <v>56</v>
+      </c>
       <c r="D10" s="6"/>
       <c r="E10" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F10" s="8"/>
+      <c r="F10" s="8" t="s">
+        <v>57</v>
+      </c>
       <c r="G10" s="3"/>
       <c r="H10" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="I10" s="5"/>
+      <c r="I10" s="5" t="s">
+        <v>58</v>
+      </c>
       <c r="J10" s="6"/>
       <c r="K10" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="L10" s="8"/>
+      <c r="L10" s="8" t="s">
+        <v>59</v>
+      </c>
       <c r="M10" s="3"/>
       <c r="N10" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="O10" s="5"/>
+      <c r="O10" s="5" t="s">
+        <v>60</v>
+      </c>
       <c r="P10" s="6"/>
       <c r="Q10" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="R10" s="8"/>
+      <c r="R10" s="8" t="s">
+        <v>61</v>
+      </c>
       <c r="S10" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="T10" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="U10" s="5"/>
+      <c r="U10" s="5" t="s">
+        <v>62</v>
+      </c>
       <c r="V10" s="6"/>
       <c r="W10" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="X10" s="8"/>
+      <c r="X10" s="8" t="s">
+        <v>63</v>
+      </c>
       <c r="Y10" s="1"/>
       <c r="Z10" s="1"/>
     </row>
@@ -1143,10 +1282,10 @@
         <v>24</v>
       </c>
       <c r="L11" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M11" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="N11" s="10">
         <v>22</v>
@@ -1179,7 +1318,7 @@
         <v>9</v>
       </c>
       <c r="X11" s="11">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="Y11" s="1"/>
       <c r="Z11" s="1"/>
@@ -1217,44 +1356,60 @@
       <c r="B13" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C13" s="5"/>
+      <c r="C13" s="5" t="s">
+        <v>64</v>
+      </c>
       <c r="D13" s="6"/>
       <c r="E13" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F13" s="8"/>
+      <c r="F13" s="8" t="s">
+        <v>65</v>
+      </c>
       <c r="G13" s="3"/>
       <c r="H13" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="I13" s="5"/>
+      <c r="I13" s="5" t="s">
+        <v>66</v>
+      </c>
       <c r="J13" s="6"/>
       <c r="K13" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="L13" s="8"/>
+      <c r="L13" s="8" t="s">
+        <v>67</v>
+      </c>
       <c r="M13" s="3"/>
       <c r="N13" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="O13" s="5"/>
+      <c r="O13" s="5" t="s">
+        <v>68</v>
+      </c>
       <c r="P13" s="6"/>
       <c r="Q13" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="R13" s="8"/>
+      <c r="R13" s="8" t="s">
+        <v>69</v>
+      </c>
       <c r="S13" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="T13" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="U13" s="5"/>
+      <c r="U13" s="5" t="s">
+        <v>70</v>
+      </c>
       <c r="V13" s="6"/>
       <c r="W13" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="X13" s="8"/>
+      <c r="X13" s="8" t="s">
+        <v>71</v>
+      </c>
       <c r="Y13" s="1"/>
       <c r="Z13" s="1"/>
     </row>
@@ -1267,7 +1422,7 @@
       </c>
       <c r="C14" s="11"/>
       <c r="D14" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E14" s="10">
         <v>9</v>
@@ -1276,7 +1431,7 @@
         <v>54</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H14" s="10">
         <v>54</v>
@@ -1316,7 +1471,7 @@
         <v>8</v>
       </c>
       <c r="U14" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="V14" s="9" t="s">
         <v>6</v>
@@ -1361,44 +1516,60 @@
       <c r="B16" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C16" s="5"/>
+      <c r="C16" s="5" t="s">
+        <v>72</v>
+      </c>
       <c r="D16" s="6"/>
       <c r="E16" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F16" s="8"/>
+      <c r="F16" s="8" t="s">
+        <v>73</v>
+      </c>
       <c r="G16" s="3"/>
       <c r="H16" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="I16" s="5"/>
+      <c r="I16" s="5" t="s">
+        <v>74</v>
+      </c>
       <c r="J16" s="6"/>
       <c r="K16" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="L16" s="8"/>
+      <c r="L16" s="8" t="s">
+        <v>75</v>
+      </c>
       <c r="M16" s="3"/>
       <c r="N16" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="O16" s="5"/>
+      <c r="O16" s="5" t="s">
+        <v>76</v>
+      </c>
       <c r="P16" s="6"/>
       <c r="Q16" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="R16" s="8"/>
+      <c r="R16" s="8" t="s">
+        <v>77</v>
+      </c>
       <c r="S16" s="3"/>
       <c r="T16" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="U16" s="5"/>
+      <c r="U16" s="5" t="s">
+        <v>78</v>
+      </c>
       <c r="V16" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="W16" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="X16" s="8"/>
+      <c r="X16" s="8" t="s">
+        <v>79</v>
+      </c>
       <c r="Y16" s="1"/>
       <c r="Z16" s="1"/>
     </row>
@@ -1440,7 +1611,7 @@
         <v>19</v>
       </c>
       <c r="O17" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P17" s="9" t="s">
         <v>3</v>
@@ -1501,27 +1672,37 @@
       <c r="B19" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C19" s="5"/>
+      <c r="C19" s="5" t="s">
+        <v>80</v>
+      </c>
       <c r="D19" s="6"/>
       <c r="E19" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F19" s="8"/>
+      <c r="F19" s="8" t="s">
+        <v>81</v>
+      </c>
       <c r="G19" s="3"/>
       <c r="H19" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="I19" s="5"/>
+      <c r="I19" s="5" t="s">
+        <v>82</v>
+      </c>
       <c r="J19" s="6"/>
       <c r="K19" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="L19" s="8"/>
+      <c r="L19" s="8" t="s">
+        <v>83</v>
+      </c>
       <c r="M19" s="3"/>
       <c r="N19" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="O19" s="5"/>
+      <c r="O19" s="5" t="s">
+        <v>84</v>
+      </c>
       <c r="P19" s="6"/>
       <c r="Q19" s="7" t="s">
         <v>2</v>
@@ -1542,12 +1723,14 @@
     </row>
     <row r="20" spans="1:26" ht="13" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C20" s="11"/>
+        <v>5</v>
+      </c>
+      <c r="B20" s="10">
+        <v>37</v>
+      </c>
+      <c r="C20" s="11">
+        <v>24</v>
+      </c>
       <c r="D20" s="9" t="s">
         <v>6</v>
       </c>
@@ -1572,7 +1755,7 @@
       </c>
       <c r="L20" s="11"/>
       <c r="M20" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="N20" s="10">
         <v>83</v>
@@ -28928,6 +29111,13 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="R2:W3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:H5"/>
+    <mergeCell ref="I4:K5"/>
+    <mergeCell ref="L4:N5"/>
+    <mergeCell ref="O4:Q5"/>
+    <mergeCell ref="R4:W5"/>
     <mergeCell ref="C1:H1"/>
     <mergeCell ref="I1:K1"/>
     <mergeCell ref="L1:N1"/>
@@ -28937,13 +29127,6 @@
     <mergeCell ref="I2:K3"/>
     <mergeCell ref="L2:N3"/>
     <mergeCell ref="O2:Q3"/>
-    <mergeCell ref="R2:W3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:H5"/>
-    <mergeCell ref="I4:K5"/>
-    <mergeCell ref="L4:N5"/>
-    <mergeCell ref="O4:Q5"/>
-    <mergeCell ref="R4:W5"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
@@ -28958,7 +29141,7 @@
   </sheetPr>
   <dimension ref="A1:C101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+    <sheetView topLeftCell="A85" workbookViewId="0">
       <selection activeCell="B98" sqref="B98"/>
     </sheetView>
   </sheetViews>
@@ -28985,7 +29168,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -28999,7 +29182,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -29023,7 +29206,7 @@
         <v>7</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -29031,7 +29214,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -29039,7 +29222,7 @@
         <v>9</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -29047,7 +29230,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -29061,7 +29244,7 @@
         <v>12</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -29081,7 +29264,7 @@
         <v>15</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -29094,7 +29277,7 @@
         <v>17</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
@@ -29108,7 +29291,7 @@
         <v>19</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
@@ -29127,7 +29310,7 @@
         <v>22</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
@@ -29135,7 +29318,7 @@
         <v>23</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
@@ -29143,10 +29326,10 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
@@ -29164,7 +29347,7 @@
         <v>27</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
@@ -29172,7 +29355,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C30" s="12"/>
     </row>
@@ -29201,10 +29384,10 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
@@ -29227,7 +29410,7 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
@@ -29250,7 +29433,7 @@
         <v>41</v>
       </c>
       <c r="C43" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
@@ -29258,7 +29441,7 @@
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C44" s="12"/>
     </row>
@@ -29322,7 +29505,7 @@
         <v>54</v>
       </c>
       <c r="C56" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
@@ -29455,7 +29638,7 @@
         <v>80</v>
       </c>
       <c r="B82" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
@@ -29473,7 +29656,7 @@
         <v>83</v>
       </c>
       <c r="B85" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
@@ -29537,7 +29720,7 @@
         <v>95</v>
       </c>
       <c r="B97" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">

</xml_diff>